<commit_message>
added excel data in excel file
</commit_message>
<xml_diff>
--- a/data/Hardware_Product_Data.xlsx
+++ b/data/Hardware_Product_Data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MBA\Internship\Telecom_Provider_Company_GenAI_Chatbot\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E1B0C3-3747-43BF-A20C-45B8307CC9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-28920" yWindow="855" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="231">
   <si>
     <t>ProductID</t>
   </si>
@@ -119,13 +125,601 @@
   </si>
   <si>
     <t>Lifetime</t>
+  </si>
+  <si>
+    <t>H106</t>
+  </si>
+  <si>
+    <t>Industrial Ethernet Switch</t>
+  </si>
+  <si>
+    <t>IES-2400</t>
+  </si>
+  <si>
+    <t>1800-555-1239</t>
+  </si>
+  <si>
+    <t>5 Years</t>
+  </si>
+  <si>
+    <t>H107</t>
+  </si>
+  <si>
+    <t>Dual-Band Router</t>
+  </si>
+  <si>
+    <t>RTR-AC1200</t>
+  </si>
+  <si>
+    <t>1800-555-1240</t>
+  </si>
+  <si>
+    <t>H108</t>
+  </si>
+  <si>
+    <t>VoIP Gateway</t>
+  </si>
+  <si>
+    <t>Gateway</t>
+  </si>
+  <si>
+    <t>VGW-3100</t>
+  </si>
+  <si>
+    <t>1800-555-1241</t>
+  </si>
+  <si>
+    <t>H109</t>
+  </si>
+  <si>
+    <t>Fiber Patch Cord</t>
+  </si>
+  <si>
+    <t>FPC-2M</t>
+  </si>
+  <si>
+    <t>1800-555-1242</t>
+  </si>
+  <si>
+    <t>H110</t>
+  </si>
+  <si>
+    <t>Wireless Access Point</t>
+  </si>
+  <si>
+    <t>Access Point</t>
+  </si>
+  <si>
+    <t>WAP-2200</t>
+  </si>
+  <si>
+    <t>1800-555-1243</t>
+  </si>
+  <si>
+    <t>H111</t>
+  </si>
+  <si>
+    <t>Business Router</t>
+  </si>
+  <si>
+    <t>BR-5000</t>
+  </si>
+  <si>
+    <t>1800-555-1244</t>
+  </si>
+  <si>
+    <t>H112</t>
+  </si>
+  <si>
+    <t>Outdoor Wi-Fi Antenna</t>
+  </si>
+  <si>
+    <t>Antenna</t>
+  </si>
+  <si>
+    <t>OWA-700</t>
+  </si>
+  <si>
+    <t>1800-555-1245</t>
+  </si>
+  <si>
+    <t>H113</t>
+  </si>
+  <si>
+    <t>SFP Transceiver Module</t>
+  </si>
+  <si>
+    <t>Transceiver</t>
+  </si>
+  <si>
+    <t>SFP-TX10</t>
+  </si>
+  <si>
+    <t>1800-555-1246</t>
+  </si>
+  <si>
+    <t>H114</t>
+  </si>
+  <si>
+    <t>Rack Mount Kit</t>
+  </si>
+  <si>
+    <t>Accessory</t>
+  </si>
+  <si>
+    <t>RMK-19</t>
+  </si>
+  <si>
+    <t>1800-555-1247</t>
+  </si>
+  <si>
+    <t>H115</t>
+  </si>
+  <si>
+    <t>Power over Ethernet Switch</t>
+  </si>
+  <si>
+    <t>PoE-24P</t>
+  </si>
+  <si>
+    <t>1800-555-1248</t>
+  </si>
+  <si>
+    <t>H116</t>
+  </si>
+  <si>
+    <t>Mesh Wi-Fi System</t>
+  </si>
+  <si>
+    <t>MESH-3PK</t>
+  </si>
+  <si>
+    <t>1800-555-1249</t>
+  </si>
+  <si>
+    <t>H117</t>
+  </si>
+  <si>
+    <t>Network Cabinet</t>
+  </si>
+  <si>
+    <t>Rack</t>
+  </si>
+  <si>
+    <t>NC-42U</t>
+  </si>
+  <si>
+    <t>1800-555-1250</t>
+  </si>
+  <si>
+    <t>H118</t>
+  </si>
+  <si>
+    <t>Media Converter</t>
+  </si>
+  <si>
+    <t>Converter</t>
+  </si>
+  <si>
+    <t>MC-GE100</t>
+  </si>
+  <si>
+    <t>1800-555-1251</t>
+  </si>
+  <si>
+    <t>H119</t>
+  </si>
+  <si>
+    <t>CAT6 Ethernet Cable</t>
+  </si>
+  <si>
+    <t>CAT6-10M</t>
+  </si>
+  <si>
+    <t>1800-555-1252</t>
+  </si>
+  <si>
+    <t>H120</t>
+  </si>
+  <si>
+    <t>4G LTE Router</t>
+  </si>
+  <si>
+    <t>LTE-R100</t>
+  </si>
+  <si>
+    <t>1800-555-1253</t>
+  </si>
+  <si>
+    <t>H121</t>
+  </si>
+  <si>
+    <t>Fiber Distribution Hub</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>FDH-12P</t>
+  </si>
+  <si>
+    <t>1800-555-1254</t>
+  </si>
+  <si>
+    <t>H122</t>
+  </si>
+  <si>
+    <t>Patch Panel 24-Port</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>PP-24</t>
+  </si>
+  <si>
+    <t>1800-555-1255</t>
+  </si>
+  <si>
+    <t>H123</t>
+  </si>
+  <si>
+    <t>Smart Switch 16-Port</t>
+  </si>
+  <si>
+    <t>SS-16P</t>
+  </si>
+  <si>
+    <t>1800-555-1256</t>
+  </si>
+  <si>
+    <t>H124</t>
+  </si>
+  <si>
+    <t>10G Network Card</t>
+  </si>
+  <si>
+    <t>NIC-10G</t>
+  </si>
+  <si>
+    <t>1800-555-1257</t>
+  </si>
+  <si>
+    <t>H125</t>
+  </si>
+  <si>
+    <t>High-Speed Powerline Kit</t>
+  </si>
+  <si>
+    <t>Adapter</t>
+  </si>
+  <si>
+    <t>PLK-600</t>
+  </si>
+  <si>
+    <t>1800-555-1258</t>
+  </si>
+  <si>
+    <t>H126</t>
+  </si>
+  <si>
+    <t>Data Center Switch</t>
+  </si>
+  <si>
+    <t>DCS-9500</t>
+  </si>
+  <si>
+    <t>1800-555-1259</t>
+  </si>
+  <si>
+    <t>H127</t>
+  </si>
+  <si>
+    <t>Wireless Bridge</t>
+  </si>
+  <si>
+    <t>WB-1500</t>
+  </si>
+  <si>
+    <t>1800-555-1260</t>
+  </si>
+  <si>
+    <t>H128</t>
+  </si>
+  <si>
+    <t>Fiber Wall Outlet</t>
+  </si>
+  <si>
+    <t>Outlet</t>
+  </si>
+  <si>
+    <t>FWO-1P</t>
+  </si>
+  <si>
+    <t>1800-555-1261</t>
+  </si>
+  <si>
+    <t>H129</t>
+  </si>
+  <si>
+    <t>UPS for Network Devices</t>
+  </si>
+  <si>
+    <t>UPS-900</t>
+  </si>
+  <si>
+    <t>1800-555-1262</t>
+  </si>
+  <si>
+    <t>H130</t>
+  </si>
+  <si>
+    <t>Signal Booster</t>
+  </si>
+  <si>
+    <t>Booster</t>
+  </si>
+  <si>
+    <t>SB-700</t>
+  </si>
+  <si>
+    <t>1800-555-1263</t>
+  </si>
+  <si>
+    <t>H131</t>
+  </si>
+  <si>
+    <t>Network Monitoring Tool</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>NMT-2025</t>
+  </si>
+  <si>
+    <t>1800-555-1264</t>
+  </si>
+  <si>
+    <t>H132</t>
+  </si>
+  <si>
+    <t>Optical Line Terminal</t>
+  </si>
+  <si>
+    <t>OLT-1600</t>
+  </si>
+  <si>
+    <t>1800-555-1265</t>
+  </si>
+  <si>
+    <t>H133</t>
+  </si>
+  <si>
+    <t>Optical Network Terminal</t>
+  </si>
+  <si>
+    <t>ONT-200</t>
+  </si>
+  <si>
+    <t>1800-555-1266</t>
+  </si>
+  <si>
+    <t>H134</t>
+  </si>
+  <si>
+    <t>Network Tester</t>
+  </si>
+  <si>
+    <t>NTEST-100</t>
+  </si>
+  <si>
+    <t>1800-555-1267</t>
+  </si>
+  <si>
+    <t>H135</t>
+  </si>
+  <si>
+    <t>Cable Organizer</t>
+  </si>
+  <si>
+    <t>CBL-ORG</t>
+  </si>
+  <si>
+    <t>1800-555-1268</t>
+  </si>
+  <si>
+    <t>H136</t>
+  </si>
+  <si>
+    <t>Patch Cord Organizer</t>
+  </si>
+  <si>
+    <t>PCO-25</t>
+  </si>
+  <si>
+    <t>1800-555-1269</t>
+  </si>
+  <si>
+    <t>H137</t>
+  </si>
+  <si>
+    <t>LAN Surge Protector</t>
+  </si>
+  <si>
+    <t>SP-LAN</t>
+  </si>
+  <si>
+    <t>1800-555-1270</t>
+  </si>
+  <si>
+    <t>H138</t>
+  </si>
+  <si>
+    <t>5G Outdoor Router</t>
+  </si>
+  <si>
+    <t>5G-OR100</t>
+  </si>
+  <si>
+    <t>1800-555-1271</t>
+  </si>
+  <si>
+    <t>H139</t>
+  </si>
+  <si>
+    <t>FTTH Drop Cable</t>
+  </si>
+  <si>
+    <t>FTTH-DROP</t>
+  </si>
+  <si>
+    <t>1800-555-1272</t>
+  </si>
+  <si>
+    <t>H140</t>
+  </si>
+  <si>
+    <t>2-Port Fiber Adapter Plate</t>
+  </si>
+  <si>
+    <t>FAP-2P</t>
+  </si>
+  <si>
+    <t>1800-555-1273</t>
+  </si>
+  <si>
+    <t>H141</t>
+  </si>
+  <si>
+    <t>Power Splitter for Modem</t>
+  </si>
+  <si>
+    <t>PS-12V</t>
+  </si>
+  <si>
+    <t>1800-555-1274</t>
+  </si>
+  <si>
+    <t>H142</t>
+  </si>
+  <si>
+    <t>USB Wi-Fi Adapter</t>
+  </si>
+  <si>
+    <t>USB-W600</t>
+  </si>
+  <si>
+    <t>1800-555-1275</t>
+  </si>
+  <si>
+    <t>H143</t>
+  </si>
+  <si>
+    <t>DOCSIS 3.1 Cable Modem</t>
+  </si>
+  <si>
+    <t>DOCSIS-MX</t>
+  </si>
+  <si>
+    <t>1800-555-1276</t>
+  </si>
+  <si>
+    <t>H144</t>
+  </si>
+  <si>
+    <t>Network Cable Tester Kit</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>NCT-KIT</t>
+  </si>
+  <si>
+    <t>1800-555-1277</t>
+  </si>
+  <si>
+    <t>H145</t>
+  </si>
+  <si>
+    <t>Telco Fiber Splice Tray</t>
+  </si>
+  <si>
+    <t>FST-12</t>
+  </si>
+  <si>
+    <t>1800-555-1278</t>
+  </si>
+  <si>
+    <t>H146</t>
+  </si>
+  <si>
+    <t>Wall Mount for Router</t>
+  </si>
+  <si>
+    <t>WM-RTR</t>
+  </si>
+  <si>
+    <t>1800-555-1279</t>
+  </si>
+  <si>
+    <t>H147</t>
+  </si>
+  <si>
+    <t>PoE Injector</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>POE-INJ</t>
+  </si>
+  <si>
+    <t>1800-555-1280</t>
+  </si>
+  <si>
+    <t>H148</t>
+  </si>
+  <si>
+    <t>Cloud-Managed Router</t>
+  </si>
+  <si>
+    <t>CM-RTR500</t>
+  </si>
+  <si>
+    <t>1800-555-1281</t>
+  </si>
+  <si>
+    <t>H149</t>
+  </si>
+  <si>
+    <t>Cable Crimping Tool</t>
+  </si>
+  <si>
+    <t>CT-500</t>
+  </si>
+  <si>
+    <t>1800-555-1282</t>
+  </si>
+  <si>
+    <t>H150</t>
+  </si>
+  <si>
+    <t>Network Wall Plate</t>
+  </si>
+  <si>
+    <t>NWP-2P</t>
+  </si>
+  <si>
+    <t>1800-555-1283</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,7 +744,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -158,29 +752,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -188,13 +770,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -232,7 +822,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -266,6 +856,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -300,9 +891,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -475,14 +1067,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="36.26953125" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" customWidth="1"/>
+    <col min="5" max="5" width="35.453125" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,103 +1104,1003 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="F51" s="2" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>